<commit_message>
update topology and addressing table
</commit_message>
<xml_diff>
--- a/IP Addressing Table.xlsx
+++ b/IP Addressing Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="181">
   <si>
     <t>Bjorn IT Solutions</t>
   </si>
@@ -555,6 +555,18 @@
   </si>
   <si>
     <t>192.168.1.198</t>
+  </si>
+  <si>
+    <t>Wireless Router</t>
+  </si>
+  <si>
+    <t>192.168.1.201</t>
+  </si>
+  <si>
+    <t>LAN</t>
+  </si>
+  <si>
+    <t>192.168.1.202</t>
   </si>
 </sst>
 </file>
@@ -590,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -618,7 +630,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -934,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I154"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,47 +970,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1012,7 +1030,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="10" t="s">
         <v>164</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1038,7 +1056,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1062,7 +1080,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1086,7 +1104,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1110,7 +1128,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1134,56 +1152,53 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A11" s="10"/>
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>178</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="E11" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="2"/>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>21</v>
@@ -1196,12 +1211,12 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>21</v>
@@ -1214,106 +1229,100 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="D16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="3" t="s">
+      <c r="H16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="E17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="3" t="s">
+      <c r="I17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="2" t="s">
+      <c r="D18" s="3"/>
+      <c r="E18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="H18" s="3"/>
+      <c r="I18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>21</v>
@@ -1321,17 +1330,23 @@
       <c r="E19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
+      <c r="G19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>165</v>
+        <v>41</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>21</v>
@@ -1344,12 +1359,12 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>21</v>
@@ -1362,106 +1377,100 @@
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="D23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="3" t="s">
+      <c r="H23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="E24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="3" t="s">
+      <c r="I24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="D25" s="3"/>
+      <c r="E25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="H25" s="3"/>
+      <c r="I25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>21</v>
@@ -1469,17 +1478,23 @@
       <c r="E26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="2"/>
+      <c r="G26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>167</v>
+        <v>42</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>21</v>
@@ -1492,12 +1507,12 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>173</v>
+        <v>13</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>21</v>
@@ -1510,130 +1525,124 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="3" t="s">
+      <c r="E30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="3" t="s">
+      <c r="I30" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="3" t="s">
+      <c r="E31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="3" t="s">
+      <c r="I31" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="D32" s="3"/>
+      <c r="E32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="3"/>
-      <c r="I31" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="3" t="s">
+      <c r="H32" s="3"/>
+      <c r="I32" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="7" t="s">
+      <c r="E33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="I33" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>166</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>21</v>
@@ -1641,17 +1650,23 @@
       <c r="E34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="2"/>
+      <c r="G34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>21</v>
@@ -1664,12 +1679,12 @@
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>21</v>
@@ -1682,187 +1697,191 @@
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="3" t="s">
+      <c r="D38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="3" t="s">
+      <c r="H38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" s="3" t="s">
+      <c r="E39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="3" t="s">
+      <c r="I39" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="2" t="s">
+      <c r="D40" s="3"/>
+      <c r="E40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H39" s="3"/>
-      <c r="I39" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="H40" s="3"/>
+      <c r="I40" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="B42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="B43" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9" t="s">
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="E43" s="9"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9" t="s">
+      <c r="E45" s="12"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="E44" s="9"/>
-    </row>
-    <row r="45" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>58</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>46</v>
@@ -1879,7 +1898,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>46</v>
@@ -1896,7 +1915,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>46</v>
@@ -1913,7 +1932,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>46</v>
@@ -1930,7 +1949,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>46</v>
@@ -1947,7 +1966,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>46</v>
@@ -1964,7 +1983,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>46</v>
@@ -1981,7 +2000,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>46</v>
@@ -1998,7 +2017,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>46</v>
@@ -2015,7 +2034,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>46</v>
@@ -2032,7 +2051,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>46</v>
@@ -2049,7 +2068,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>46</v>
@@ -2066,7 +2085,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>46</v>
@@ -2075,15 +2094,15 @@
         <v>68</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>46</v>
@@ -2092,15 +2111,15 @@
         <v>68</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>46</v>
@@ -2117,7 +2136,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>46</v>
@@ -2134,7 +2153,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>46</v>
@@ -2151,7 +2170,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>46</v>
@@ -2168,7 +2187,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>46</v>
@@ -2183,86 +2202,86 @@
         <v>31</v>
       </c>
     </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="4"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="9" t="s">
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="E69" s="9"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="8"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="9" t="s">
+      <c r="E71" s="12"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="E70" s="9"/>
-    </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="E72" s="12"/>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E73" s="6" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>79</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E72" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>80</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E73" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>46</v>
@@ -2279,7 +2298,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>46</v>
@@ -2296,7 +2315,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>46</v>
@@ -2313,7 +2332,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>46</v>
@@ -2330,7 +2349,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>46</v>
@@ -2347,7 +2366,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>46</v>
@@ -2364,7 +2383,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>46</v>
@@ -2381,7 +2400,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>46</v>
@@ -2398,7 +2417,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>46</v>
@@ -2415,7 +2434,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>46</v>
@@ -2432,7 +2451,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>46</v>
@@ -2449,7 +2468,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>46</v>
@@ -2466,7 +2485,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>46</v>
@@ -2475,15 +2494,15 @@
         <v>68</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E86" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>46</v>
@@ -2492,15 +2511,15 @@
         <v>68</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E87" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>46</v>
@@ -2517,7 +2536,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>46</v>
@@ -2532,80 +2551,80 @@
         <v>37</v>
       </c>
     </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>95</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E90" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
+      <c r="A91" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E91" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="9" t="s">
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="E91" s="9"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="8"/>
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="9" t="s">
+      <c r="E93" s="12"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="E92" s="9"/>
-    </row>
-    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="E94" s="12"/>
+    </row>
+    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D95" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E93" s="6" t="s">
+      <c r="E95" s="6" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>98</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D94" t="s">
-        <v>38</v>
-      </c>
-      <c r="E94" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>99</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D95" t="s">
-        <v>38</v>
-      </c>
-      <c r="E95" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>46</v>
@@ -2622,7 +2641,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>46</v>
@@ -2639,7 +2658,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>46</v>
@@ -2656,7 +2675,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>46</v>
@@ -2673,7 +2692,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>46</v>
@@ -2690,7 +2709,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>46</v>
@@ -2707,7 +2726,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>46</v>
@@ -2724,7 +2743,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>46</v>
@@ -2741,7 +2760,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>46</v>
@@ -2758,7 +2777,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>46</v>
@@ -2775,7 +2794,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>46</v>
@@ -2792,7 +2811,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>46</v>
@@ -2809,7 +2828,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>46</v>
@@ -2826,7 +2845,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>46</v>
@@ -2843,7 +2862,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>46</v>
@@ -2860,7 +2879,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>46</v>
@@ -2877,7 +2896,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>46</v>
@@ -2894,7 +2913,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>46</v>
@@ -2911,7 +2930,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>46</v>
@@ -2928,7 +2947,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>46</v>
@@ -2945,7 +2964,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>46</v>
@@ -2962,7 +2981,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>46</v>
@@ -2979,7 +2998,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>46</v>
@@ -2996,7 +3015,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>46</v>
@@ -3013,7 +3032,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>46</v>
@@ -3030,7 +3049,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>46</v>
@@ -3047,7 +3066,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>46</v>
@@ -3064,7 +3083,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>46</v>
@@ -3081,7 +3100,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>46</v>
@@ -3090,15 +3109,15 @@
         <v>68</v>
       </c>
       <c r="D124" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E124" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>46</v>
@@ -3107,15 +3126,15 @@
         <v>68</v>
       </c>
       <c r="D125" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E125" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>46</v>
@@ -3132,7 +3151,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>46</v>
@@ -3149,7 +3168,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>46</v>
@@ -3166,7 +3185,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>46</v>
@@ -3181,80 +3200,80 @@
         <v>39</v>
       </c>
     </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>132</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D130" t="s">
+        <v>34</v>
+      </c>
+      <c r="E130" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="8" t="s">
+      <c r="A131" t="s">
+        <v>133</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D131" t="s">
+        <v>34</v>
+      </c>
+      <c r="E131" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B131" s="8"/>
-      <c r="C131" s="8"/>
-      <c r="D131" s="9" t="s">
+      <c r="B133" s="10"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="E131" s="9"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="8"/>
-      <c r="B132" s="8"/>
-      <c r="C132" s="8"/>
-      <c r="D132" s="9" t="s">
+      <c r="E133" s="12"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="10"/>
+      <c r="B134" s="10"/>
+      <c r="C134" s="10"/>
+      <c r="D134" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="E132" s="9"/>
-    </row>
-    <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+      <c r="E134" s="12"/>
+    </row>
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B135" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C135" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D133" s="1" t="s">
+      <c r="D135" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E133" s="6" t="s">
+      <c r="E135" s="6" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>135</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D134" t="s">
-        <v>33</v>
-      </c>
-      <c r="E134" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>137</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D135" t="s">
-        <v>33</v>
-      </c>
-      <c r="E135" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>46</v>
@@ -3271,7 +3290,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>46</v>
@@ -3288,7 +3307,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>46</v>
@@ -3305,7 +3324,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>46</v>
@@ -3322,7 +3341,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>46</v>
@@ -3339,7 +3358,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>46</v>
@@ -3356,7 +3375,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>46</v>
@@ -3373,7 +3392,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>46</v>
@@ -3390,7 +3409,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>46</v>
@@ -3407,7 +3426,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>46</v>
@@ -3424,7 +3443,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>46</v>
@@ -3441,7 +3460,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>46</v>
@@ -3458,7 +3477,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>46</v>
@@ -3467,15 +3486,15 @@
         <v>68</v>
       </c>
       <c r="D148" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E148" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>46</v>
@@ -3484,15 +3503,15 @@
         <v>68</v>
       </c>
       <c r="D149" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E149" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>46</v>
@@ -3509,7 +3528,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>46</v>
@@ -3526,7 +3545,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>46</v>
@@ -3543,7 +3562,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>46</v>
@@ -3560,7 +3579,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>46</v>
@@ -3575,29 +3594,64 @@
         <v>44</v>
       </c>
     </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D155" t="s">
+        <v>34</v>
+      </c>
+      <c r="E155" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>155</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D156" t="s">
+        <v>34</v>
+      </c>
+      <c r="E156" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
+  <dataConsolidate/>
   <mergeCells count="21">
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A25:A32"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="A131:C132"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="A91:C92"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="A69:C70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="A43:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="A133:C134"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="A93:C94"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="A71:C72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="A45:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A26:A33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>